<commit_message>
Added data to the script
</commit_message>
<xml_diff>
--- a/Parfume_prices_database.xlsx
+++ b/Parfume_prices_database.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -35,6 +36,10 @@
       <sz val="14"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -50,7 +55,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -73,18 +78,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="DateStyle" xfId="1"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,13 +440,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:G11"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="89.42578125" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
@@ -466,7 +485,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Strona</t>
+          <t>Data</t>
         </is>
       </c>
     </row>
@@ -797,6 +816,236 @@
       <c r="F12" t="inlineStr">
         <is>
           <t>https://www.notino.pl/hugo-boss/boss-bottled-night-woda-toaletowa-dla-mczyzn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Urban Hero Gold </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 ml </t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>144.5</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/jimmy-choo/urban-hero-gold-woda-perfumowana-dla-mezczyzn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Urban Hero Gold </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 ml </t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>144.5</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/jimmy-choo/urban-hero-gold-woda-perfumowana-dla-mezczyzn/</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="n">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Urban Hero Gold </t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 ml </t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>144.5</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/jimmy-choo/urban-hero-gold-woda-perfumowana-dla-mezczyzn/</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="n">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Urban Hero Gold </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 ml </t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>144.5</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/jimmy-choo/urban-hero-gold-woda-perfumowana-dla-mezczyzn/</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="n">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Urban Hero Gold </t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 ml </t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>144.5</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/jimmy-choo/urban-hero-gold-woda-perfumowana-dla-mezczyzn/</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="n">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Urban Hero Gold </t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 ml </t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>144.5</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/jimmy-choo/urban-hero-gold-woda-perfumowana-dla-mezczyzn/</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="n">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Urban Hero Gold </t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 ml </t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>144.5</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/jimmy-choo/urban-hero-gold-woda-perfumowana-dla-mezczyzn/</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>04.03.2023</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
almost whole app done
</commit_message>
<xml_diff>
--- a/Parfume_prices_database.xlsx
+++ b/Parfume_prices_database.xlsx
@@ -440,10 +440,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -455,12 +455,12 @@
     <row r="1" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Marka</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Produkt</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Marka</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -492,12 +492,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t xml:space="preserve">Urban Hero Gold </t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Jimmy Choo</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -525,12 +525,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Guy Laroche</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t xml:space="preserve">Drakkar Noir </t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Guy Laroche</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -558,12 +558,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Guy Laroche</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t xml:space="preserve">DRAKKAR INTENSE </t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Guy Laroche</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -591,12 +591,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Karl Lagerfeld</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t xml:space="preserve">Lagerfeld Classic Grey </t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Karl Lagerfeld</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -624,12 +624,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Karl Lagerfeld</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t xml:space="preserve">Lagerfeld Classic </t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Karl Lagerfeld</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -657,12 +657,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Karl Lagerfeld</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t xml:space="preserve">Bois De Cèdre </t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Karl Lagerfeld</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -690,12 +690,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Versace</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t xml:space="preserve">Eros </t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Versace</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -723,12 +723,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Versace</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t xml:space="preserve">Eros </t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Versace</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -756,12 +756,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Versace</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t xml:space="preserve">Eros Flame </t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Versace</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -789,12 +789,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Hugo Boss</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t xml:space="preserve">BOSS Bottled Night </t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Hugo Boss</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -822,12 +822,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Hugo Boss</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t xml:space="preserve">BOSS Bottled Night </t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Hugo Boss</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -855,12 +855,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t xml:space="preserve">Urban Hero Gold </t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Jimmy Choo</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -888,12 +888,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t xml:space="preserve">Urban Hero Gold </t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Jimmy Choo</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -921,12 +921,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Guy Laroche</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t xml:space="preserve">Drakkar Noir </t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Guy Laroche</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -954,12 +954,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Guy Laroche</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t xml:space="preserve">DRAKKAR INTENSE </t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Guy Laroche</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -987,12 +987,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>Karl Lagerfeld</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t xml:space="preserve">Lagerfeld Classic Grey </t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Karl Lagerfeld</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1020,12 +1020,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Karl Lagerfeld</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t xml:space="preserve">Lagerfeld Classic </t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Karl Lagerfeld</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1053,12 +1053,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>Karl Lagerfeld</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t xml:space="preserve">Bois De Cèdre </t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Karl Lagerfeld</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1086,12 +1086,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>Versace</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t xml:space="preserve">Eros </t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Versace</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1119,12 +1119,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>Versace</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t xml:space="preserve">Eros </t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Versace</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1152,12 +1152,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Versace</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t xml:space="preserve">Eros Flame </t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Versace</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1185,12 +1185,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>Hugo Boss</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t xml:space="preserve">BOSS Bottled Night </t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Hugo Boss</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1218,12 +1218,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>Hugo Boss</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t xml:space="preserve">BOSS Bottled Night </t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Hugo Boss</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1251,12 +1251,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t xml:space="preserve">Urban Hero Gold </t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Jimmy Choo</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1284,12 +1284,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t xml:space="preserve">Urban Hero Gold </t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Jimmy Choo</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1313,6 +1313,426 @@
       <c r="G26" t="inlineStr">
         <is>
           <t>10.03.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Urban Hero Gold </t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 ml </t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>133.5</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/jimmy-choo/urban-hero-gold-woda-perfumowana-dla-mezczyzn/</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>10.03.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Jimmy Choo</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Urban Hero Gold </t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">100 ml </t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/jimmy-choo/urban-hero-gold-woda-perfumowana-dla-mezczyzn/</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>04.04.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>JOOP!</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Homme </t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>woda toaletowa dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">200 ml </t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>196</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/joop/homme-woda-toaletowa-dla-mczyzn/p-402506/?gclid=EAIaIQobChMInZmGhfyU_gIVg9eyCh16ygIcEAQYASABEgJDUPD_BwE</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>JOOP!</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Homme </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>woda toaletowa dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">200 ml </t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>196</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/joop/homme-woda-toaletowa-dla-mczyzn/p-402506/?gclid=EAIaIQobChMInZmGhfyU_gIVg9eyCh16ygIcEAQYASABEgJDUPD_BwE</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Armani</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sì </t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla kobiet</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 ml </t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>273.28</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/armani/si-woda-perfumowana-dla-kobiet/</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>07.04.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Armani</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sì </t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla kobiet</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 ml </t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>375</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/armani/si-woda-perfumowana-dla-kobiet/</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Armani</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sì </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>woda perfumowana dla kobiet</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 ml </t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>375</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/armani/si-woda-perfumowana-dla-kobiet/</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Paco Rabanne</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Invictus Victory Elixir </t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>perfumy dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">200 ml </t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>885</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/paco-rabanne/invictus-victory-elixir-perfumy-dla-mezczyzn/p-16168428/</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Paco Rabanne</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Invictus Victory Elixir </t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>perfumy dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">200 ml </t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>885</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/paco-rabanne/invictus-victory-elixir-perfumy-dla-mezczyzn/p-16168428/</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Paco Rabanne</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Invictus Victory Elixir </t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>perfumy dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">200 ml </t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>885</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/paco-rabanne/invictus-victory-elixir-perfumy-dla-mezczyzn/p-16168428/</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Paco Rabanne</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Invictus Victory Elixir </t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>perfumy dla mężczyzn</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">200 ml </t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>885</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/paco-rabanne/invictus-victory-elixir-perfumy-dla-mezczyzn/p-16168428/</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Parfums</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Roja </t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>perfumy unisex</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">100 ml </t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>10414.8</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>https://www.notino.pl/roja-parfums/roja-perfumy-unisex/p-565038/?utm_source=cj&amp;utm_medium=affiliate&amp;utm_campaign=4023395&amp;utm_term=8280252&amp;cjevent=43e4d545d86f11ed821735220a18b8f8&amp;cjdata=MXxZfDB8WXww</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
         </is>
       </c>
     </row>

</xml_diff>